<commit_message>
FIX Error And Client Requested
</commit_message>
<xml_diff>
--- a/public/FILE_TEMPLATE.xlsx
+++ b/public/FILE_TEMPLATE.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xampp\htdocs\ppdbv2\public\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334D31D1-8838-42A3-905D-BCA1F9B00BCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
-  <si>
-    <t>DATA PENDAFTAR SMK YPE KROYA</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+  <si>
+    <t>No</t>
   </si>
   <si>
     <t>Nama Lengkap</t>
@@ -41,6 +46,9 @@
     <t>Alamat</t>
   </si>
   <si>
+    <t>No. HP</t>
+  </si>
+  <si>
     <t>Email</t>
   </si>
   <si>
@@ -57,59 +65,51 @@
   </si>
   <si>
     <t>l</t>
-  </si>
-  <si>
-    <t>sdasdsa</t>
-  </si>
-  <si>
-    <t>SMP Negeri 1 Sumpiuh</t>
-  </si>
-  <si>
-    <t>Ari pur</t>
-  </si>
-  <si>
-    <t>Purbalingga</t>
-  </si>
-  <si>
-    <t>p</t>
   </si>
   <si>
     <t>Jln Raya Tambak
 Purwodadi</t>
   </si>
   <si>
-    <t>smp n 1sumpiuh</t>
+    <t>089658176349</t>
+  </si>
+  <si>
+    <t>synystergates0210@gmail.com</t>
+  </si>
+  <si>
+    <t>SMP NEGERI 1 MAJENANG</t>
+  </si>
+  <si>
+    <t>muhammad faizar</t>
+  </si>
+  <si>
+    <t>benbruce0210@gmail.com</t>
+  </si>
+  <si>
+    <t>SMP Negeri 1 Sumpiuh</t>
+  </si>
+  <si>
+    <t>adi prasetyo</t>
+  </si>
+  <si>
+    <t>Purbalingga</t>
+  </si>
+  <si>
+    <t>synysteates0210@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -165,21 +165,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -469,132 +474,167 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A3" sqref="A3:I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.851" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="19.995" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="9.283" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="24.708" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="3" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3302080205970001</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4546545400</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3302080205870001</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2">
-        <v>4546545400</v>
-      </c>
-      <c r="C4" s="2">
-        <v>3302080205970001</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1234567895</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3302080212970001</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2">
-        <v>1234567890</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3302080212970001</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
-        <v>20</v>
+      <c r="J4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells>
-    <mergeCell ref="A1:I1"/>
-  </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>